<commit_message>
Results from July 09, 2020 06:56:48 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-09.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-09.xlsx
@@ -518,47 +518,43 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Arkansas</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
         <v>44021</v>
       </c>
       <c r="C2" t="n">
-        <v>25246</v>
+        <v>24459</v>
       </c>
       <c r="D2" t="n">
-        <v>305</v>
+        <v>703</v>
       </c>
       <c r="E2" t="n">
-        <v>5471</v>
+        <v>2821</v>
       </c>
       <c r="F2" t="n">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="G2" t="n">
-        <v>25.07</v>
+        <v>0.12</v>
       </c>
       <c r="H2" t="n">
-        <v>25.69</v>
+        <v>0.13</v>
       </c>
       <c r="I2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" t="n">
-        <v>21820</v>
-      </c>
-      <c r="L2" t="n">
-        <v>288</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
-        <v>460970</v>
+        <v>3365783</v>
       </c>
       <c r="N2" t="n">
-        <v>15.41</v>
+        <v>12.07</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -569,43 +565,47 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>Texas -- Bexar County</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C3" t="n">
-        <v>110602</v>
+        <v>17679</v>
       </c>
       <c r="D3" t="n">
-        <v>8243</v>
+        <v>165</v>
       </c>
       <c r="E3" t="n">
-        <v>10414</v>
+        <v>464</v>
       </c>
       <c r="F3" t="n">
-        <v>675</v>
+        <v>17</v>
       </c>
       <c r="G3" t="n">
-        <v>9.42</v>
+        <v>6.81</v>
       </c>
       <c r="H3" t="n">
-        <v>8.19</v>
+        <v>15.32</v>
       </c>
       <c r="I3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="b">
         <v>0</v>
       </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
+      <c r="K3" t="n">
+        <v>6812</v>
+      </c>
+      <c r="L3" t="n">
+        <v>111</v>
+      </c>
       <c r="M3" t="n">
-        <v>510558</v>
+        <v>146703</v>
       </c>
       <c r="N3" t="n">
-        <v>7.48</v>
+        <v>7.62</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -616,47 +616,51 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>New York -- New York</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44020</v>
-      </c>
-      <c r="C4" t="n">
-        <v>46424</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1032</v>
+        <v>44021</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>214952</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>18637</t>
+        </is>
       </c>
       <c r="E4" t="n">
-        <v>16007</v>
+        <v>33362</v>
       </c>
       <c r="F4" t="n">
-        <v>459</v>
+        <v>5214</v>
       </c>
       <c r="G4" t="n">
-        <v>46.01</v>
+        <v>30.15</v>
       </c>
       <c r="H4" t="n">
-        <v>46.18</v>
+        <v>30.52</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>34792</v>
+        <v>110643</v>
       </c>
       <c r="L4" t="n">
-        <v>994</v>
+        <v>17085</v>
       </c>
       <c r="M4" t="n">
-        <v>1293186</v>
+        <v>2049418</v>
       </c>
       <c r="N4" t="n">
-        <v>26.58</v>
+        <v>24.27</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -667,76 +671,94 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Iowa</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+          <t>Rhode Island</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>44015</v>
+      </c>
+      <c r="C5" t="n">
+        <v>16491</v>
+      </c>
+      <c r="D5" t="n">
+        <v>960</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1592</v>
+      </c>
+      <c r="F5" t="n">
+        <v>48</v>
+      </c>
+      <c r="G5" t="n">
+        <v>12.29</v>
+      </c>
+      <c r="H5" t="n">
+        <v>6.14</v>
+      </c>
       <c r="I5" t="b">
         <v>0</v>
       </c>
       <c r="J5" t="b">
         <v>0</v>
       </c>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
+      <c r="K5" t="n">
+        <v>12950</v>
+      </c>
+      <c r="L5" t="n">
+        <v>782</v>
+      </c>
       <c r="M5" t="n">
-        <v>109911</v>
+        <v>69254</v>
       </c>
       <c r="N5" t="n">
-        <v>3.51</v>
+        <v>6.55</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>An error occurred. ... ValueError('Unable to parse "Reported Deaths In Adair : No Data" as int')</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Illinois</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C6" t="n">
-        <v>149432</v>
+        <v>57591</v>
       </c>
       <c r="D6" t="n">
-        <v>7099</v>
+        <v>710</v>
       </c>
       <c r="E6" t="n">
-        <v>25072</v>
+        <v>11825</v>
       </c>
       <c r="F6" t="n">
-        <v>1967</v>
+        <v>249</v>
       </c>
       <c r="G6" t="n">
-        <v>16.78</v>
+        <v>20.53</v>
       </c>
       <c r="H6" t="n">
-        <v>27.71</v>
+        <v>35.07</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
       </c>
       <c r="J6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
-        <v>1824125</v>
+        <v>1117489</v>
       </c>
       <c r="N6" t="n">
-        <v>14.23</v>
+        <v>16.8</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -747,41 +769,49 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Maine</t>
+          <t>Utah</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
         <v>44021</v>
       </c>
-      <c r="C7" t="n">
-        <v>3486</v>
-      </c>
-      <c r="D7" t="n">
-        <v>111</v>
-      </c>
-      <c r="E7" t="n">
-        <v>809</v>
-      </c>
-      <c r="F7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>27356</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>205</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>704</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>&lt;5</t>
+        </is>
+      </c>
       <c r="G7" t="n">
-        <v>26.23</v>
+        <v>2.6</v>
       </c>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K7" t="n">
-        <v>3084</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="n">
-        <v>17881</v>
+        <v>35862</v>
       </c>
       <c r="N7" t="n">
-        <v>1.34</v>
+        <v>1.18</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -792,47 +822,47 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Texas -- Bexar County</t>
+          <t>Kentucky</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C8" t="n">
-        <v>16725</v>
+        <v>18245</v>
       </c>
       <c r="D8" t="n">
-        <v>146</v>
+        <v>612</v>
       </c>
       <c r="E8" t="n">
-        <v>464</v>
+        <v>1729</v>
       </c>
       <c r="F8" t="n">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="G8" t="n">
-        <v>6.81</v>
+        <v>13.88</v>
       </c>
       <c r="H8" t="n">
-        <v>15.32</v>
+        <v>15.3</v>
       </c>
       <c r="I8" t="b">
         <v>0</v>
       </c>
       <c r="J8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>6812</v>
+        <v>12461</v>
       </c>
       <c r="L8" t="n">
-        <v>111</v>
+        <v>574</v>
       </c>
       <c r="M8" t="n">
-        <v>146703</v>
+        <v>354112</v>
       </c>
       <c r="N8" t="n">
-        <v>7.62</v>
+        <v>7.98</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -843,43 +873,47 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Washington, DC</t>
+          <t>Arkansas</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>44019</v>
+        <v>44021</v>
       </c>
       <c r="C9" t="n">
-        <v>10569</v>
+        <v>26052</v>
       </c>
       <c r="D9" t="n">
-        <v>561</v>
+        <v>309</v>
       </c>
       <c r="E9" t="n">
-        <v>5241</v>
+        <v>5611</v>
       </c>
       <c r="F9" t="n">
-        <v>418</v>
+        <v>74</v>
       </c>
       <c r="G9" t="n">
-        <v>49.59</v>
+        <v>24.98</v>
       </c>
       <c r="H9" t="n">
-        <v>74.51000000000001</v>
+        <v>25.52</v>
       </c>
       <c r="I9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="b">
         <v>1</v>
       </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="K9" t="n">
+        <v>22465</v>
+      </c>
+      <c r="L9" t="n">
+        <v>290</v>
+      </c>
       <c r="M9" t="n">
-        <v>321317</v>
+        <v>460970</v>
       </c>
       <c r="N9" t="n">
-        <v>46.94</v>
+        <v>15.41</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -890,47 +924,47 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Kentucky</t>
+          <t>California - San Diego</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C10" t="n">
-        <v>17919</v>
+        <v>18402</v>
       </c>
       <c r="D10" t="n">
-        <v>608</v>
+        <v>415</v>
       </c>
       <c r="E10" t="n">
-        <v>1707</v>
+        <v>666</v>
       </c>
       <c r="F10" t="n">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="G10" t="n">
-        <v>13.77</v>
+        <v>4.54</v>
       </c>
       <c r="H10" t="n">
-        <v>15.41</v>
+        <v>3.93</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
       </c>
       <c r="J10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>12399</v>
+        <v>14668</v>
       </c>
       <c r="L10" t="n">
-        <v>570</v>
+        <v>407</v>
       </c>
       <c r="M10" t="n">
-        <v>354112</v>
+        <v>166412</v>
       </c>
       <c r="N10" t="n">
-        <v>7.98</v>
+        <v>5.04</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -941,29 +975,29 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C11" t="n">
-        <v>39589</v>
+        <v>67988</v>
       </c>
       <c r="D11" t="n">
-        <v>1485</v>
+        <v>1937</v>
       </c>
       <c r="E11" t="n">
-        <v>8083</v>
+        <v>10150</v>
       </c>
       <c r="F11" t="n">
-        <v>131</v>
+        <v>437</v>
       </c>
       <c r="G11" t="n">
-        <v>20.42</v>
+        <v>14.93</v>
       </c>
       <c r="H11" t="n">
-        <v>8.82</v>
+        <v>22.56</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
@@ -974,10 +1008,10 @@
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="n">
-        <v>342186</v>
+        <v>1613285</v>
       </c>
       <c r="N11" t="n">
-        <v>6.19</v>
+        <v>19.17</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -988,47 +1022,39 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C12" t="n">
-        <v>33154</v>
+        <v>14251</v>
       </c>
       <c r="D12" t="n">
-        <v>807</v>
+        <v>533</v>
       </c>
       <c r="E12" t="n">
-        <v>5634</v>
-      </c>
-      <c r="F12" t="n">
-        <v>192</v>
-      </c>
+        <v>270</v>
+      </c>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
-        <v>18.88</v>
-      </c>
-      <c r="H12" t="n">
-        <v>24.15</v>
-      </c>
+        <v>1.89</v>
+      </c>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="b">
-        <v>1</v>
-      </c>
-      <c r="K12" t="n">
-        <v>29848</v>
-      </c>
-      <c r="L12" t="n">
-        <v>795</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
       <c r="M12" t="n">
-        <v>368744</v>
+        <v>43006</v>
       </c>
       <c r="N12" t="n">
-        <v>6.38</v>
+        <v>2.06</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1039,43 +1065,41 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Florida -- Miami-Dade County</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C13" t="n">
-        <v>49063</v>
+        <v>55961</v>
       </c>
       <c r="D13" t="n">
-        <v>2539</v>
+        <v>1092</v>
       </c>
       <c r="E13" t="n">
-        <v>5905</v>
-      </c>
-      <c r="F13" t="n">
-        <v>368</v>
-      </c>
+        <v>6426</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
-        <v>12.04</v>
-      </c>
-      <c r="H13" t="n">
-        <v>14.49</v>
-      </c>
+        <v>20.52</v>
+      </c>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="b">
         <v>1</v>
       </c>
-      <c r="K13" t="inlineStr"/>
+      <c r="K13" t="n">
+        <v>31311</v>
+      </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="n">
-        <v>619472</v>
+        <v>481976</v>
       </c>
       <c r="N13" t="n">
-        <v>9.33</v>
+        <v>17.75</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1086,43 +1110,41 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>Florida -- Orange County</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C14" t="n">
-        <v>55986</v>
+        <v>15595</v>
       </c>
       <c r="D14" t="n">
-        <v>685</v>
+        <v>69</v>
       </c>
       <c r="E14" t="n">
-        <v>11560</v>
-      </c>
-      <c r="F14" t="n">
-        <v>241</v>
-      </c>
+        <v>2051</v>
+      </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
-        <v>20.65</v>
-      </c>
-      <c r="H14" t="n">
-        <v>35.18</v>
-      </c>
+        <v>24.65</v>
+      </c>
+      <c r="H14" t="inlineStr"/>
       <c r="I14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="b">
         <v>1</v>
       </c>
-      <c r="K14" t="inlineStr"/>
+      <c r="K14" t="n">
+        <v>8319</v>
+      </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="n">
-        <v>1117489</v>
+        <v>277193</v>
       </c>
       <c r="N14" t="n">
-        <v>16.8</v>
+        <v>20.98</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1133,51 +1155,47 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>New York -- New York</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>44020</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>214570</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>18618</t>
-        </is>
+        <v>44021</v>
+      </c>
+      <c r="C15" t="n">
+        <v>48588</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1042</v>
       </c>
       <c r="E15" t="n">
-        <v>33320</v>
+        <v>16434</v>
       </c>
       <c r="F15" t="n">
-        <v>5210</v>
+        <v>462</v>
       </c>
       <c r="G15" t="n">
-        <v>30.16</v>
+        <v>45.81</v>
       </c>
       <c r="H15" t="n">
-        <v>30.52</v>
+        <v>46.02</v>
       </c>
       <c r="I15" t="b">
         <v>0</v>
       </c>
       <c r="J15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>110482</v>
+        <v>35877</v>
       </c>
       <c r="L15" t="n">
-        <v>17070</v>
+        <v>1004</v>
       </c>
       <c r="M15" t="n">
-        <v>2049418</v>
+        <v>1293186</v>
       </c>
       <c r="N15" t="n">
-        <v>24.27</v>
+        <v>26.58</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1188,49 +1206,47 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>California - Los Angeles</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
         <v>44020</v>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>26755</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>201</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>689</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>&lt;5</t>
-        </is>
+      <c r="C16" t="n">
+        <v>124738</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3689</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3358</v>
+      </c>
+      <c r="F16" t="n">
+        <v>375</v>
       </c>
       <c r="G16" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="H16" t="inlineStr"/>
+        <v>4.75</v>
+      </c>
+      <c r="H16" t="n">
+        <v>10.92</v>
+      </c>
       <c r="I16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="b">
         <v>0</v>
       </c>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
+      <c r="K16" t="n">
+        <v>70741</v>
+      </c>
+      <c r="L16" t="n">
+        <v>3434</v>
+      </c>
       <c r="M16" t="n">
-        <v>35862</v>
+        <v>823987</v>
       </c>
       <c r="N16" t="n">
-        <v>1.18</v>
+        <v>8.16</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1241,47 +1257,47 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Vermont</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C17" t="n">
-        <v>1256</v>
+        <v>71447</v>
       </c>
       <c r="D17" t="n">
-        <v>56</v>
+        <v>3160</v>
       </c>
       <c r="E17" t="n">
-        <v>128</v>
+        <v>20515</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>1276</v>
       </c>
       <c r="G17" t="n">
-        <v>10.47</v>
+        <v>28.71</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>40.38</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
       </c>
       <c r="J17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>1223</v>
+        <v>58791</v>
       </c>
       <c r="L17" t="n">
-        <v>56</v>
+        <v>71423</v>
       </c>
       <c r="M17" t="n">
-        <v>8058</v>
+        <v>1788090</v>
       </c>
       <c r="N17" t="n">
-        <v>1.29</v>
+        <v>29.78</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1292,47 +1308,43 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Missouri</t>
+          <t>Mississippi</t>
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>44009</v>
+        <v>44020</v>
       </c>
       <c r="C18" t="n">
-        <v>20261</v>
+        <v>33591</v>
       </c>
       <c r="D18" t="n">
-        <v>996</v>
+        <v>1204</v>
       </c>
       <c r="E18" t="n">
-        <v>5758</v>
+        <v>16002</v>
       </c>
       <c r="F18" t="n">
-        <v>246</v>
+        <v>600</v>
       </c>
       <c r="G18" t="n">
-        <v>49.66</v>
+        <v>47.64</v>
       </c>
       <c r="H18" t="n">
-        <v>38.56</v>
+        <v>49.83</v>
       </c>
       <c r="I18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="b">
         <v>1</v>
       </c>
-      <c r="K18" t="n">
-        <v>11594</v>
-      </c>
-      <c r="L18" t="n">
-        <v>638</v>
-      </c>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
       <c r="M18" t="n">
-        <v>704896</v>
+        <v>1125834</v>
       </c>
       <c r="N18" t="n">
-        <v>11.57</v>
+        <v>37.67</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1343,29 +1355,29 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Pennsylvania</t>
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>44019</v>
+        <v>44021</v>
       </c>
       <c r="C19" t="n">
-        <v>289468</v>
+        <v>90202</v>
       </c>
       <c r="D19" t="n">
-        <v>6474</v>
+        <v>6848</v>
       </c>
       <c r="E19" t="n">
-        <v>8125</v>
+        <v>12101</v>
       </c>
       <c r="F19" t="n">
-        <v>582</v>
+        <v>1426</v>
       </c>
       <c r="G19" t="n">
-        <v>4.4</v>
+        <v>30.15</v>
       </c>
       <c r="H19" t="n">
-        <v>9.1</v>
+        <v>21.68</v>
       </c>
       <c r="I19" t="b">
         <v>0</v>
@@ -1374,16 +1386,16 @@
         <v>1</v>
       </c>
       <c r="K19" t="n">
-        <v>185891</v>
+        <v>40142</v>
       </c>
       <c r="L19" t="n">
-        <v>6375</v>
+        <v>6579</v>
       </c>
       <c r="M19" t="n">
-        <v>2267875</v>
+        <v>1423319</v>
       </c>
       <c r="N19" t="n">
-        <v>5.79</v>
+        <v>11.13</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -1394,26 +1406,30 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>New Mexico</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C20" t="n">
-        <v>14017</v>
+        <v>229367</v>
       </c>
       <c r="D20" t="n">
-        <v>527</v>
+        <v>4009</v>
       </c>
       <c r="E20" t="n">
-        <v>266</v>
-      </c>
-      <c r="F20" t="inlineStr"/>
+        <v>29577</v>
+      </c>
+      <c r="F20" t="n">
+        <v>789</v>
+      </c>
       <c r="G20" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="H20" t="inlineStr"/>
+        <v>12.9</v>
+      </c>
+      <c r="H20" t="n">
+        <v>19.68</v>
+      </c>
       <c r="I20" t="b">
         <v>1</v>
       </c>
@@ -1423,10 +1439,10 @@
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="n">
-        <v>43006</v>
+        <v>3316376</v>
       </c>
       <c r="N20" t="n">
-        <v>2.06</v>
+        <v>16.1</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1437,47 +1453,39 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Alaska</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C21" t="n">
-        <v>1226</v>
+        <v>1466</v>
       </c>
       <c r="D21" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E21" t="n">
-        <v>30</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="n">
-        <v>1.41</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0</v>
-      </c>
+        <v>0.41</v>
+      </c>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" t="b">
         <v>1</v>
       </c>
-      <c r="K21" t="n">
-        <v>2135</v>
-      </c>
-      <c r="L21" t="n">
-        <v>34</v>
-      </c>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
       <c r="M21" t="n">
-        <v>24129</v>
+        <v>4630</v>
       </c>
       <c r="N21" t="n">
-        <v>3.27</v>
+        <v>0.44</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -1488,62 +1496,80 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Texas</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
+          <t>Vermont</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>44021</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1272</v>
+      </c>
+      <c r="D22" t="n">
+        <v>56</v>
+      </c>
+      <c r="E22" t="n">
+        <v>136</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>10.99</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
       <c r="I22" t="b">
         <v>0</v>
       </c>
       <c r="J22" t="b">
-        <v>0</v>
-      </c>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K22" t="n">
+        <v>1238</v>
+      </c>
+      <c r="L22" t="n">
+        <v>56</v>
+      </c>
       <c r="M22" t="n">
-        <v>3365783</v>
+        <v>8058</v>
       </c>
       <c r="N22" t="n">
-        <v>12.07</v>
+        <v>1.29</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>An error occurred. ... KeyError("None of ['Race/Ethnicity'] are in the columns")</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Maryland</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C23" t="n">
-        <v>70861</v>
+        <v>35525</v>
       </c>
       <c r="D23" t="n">
-        <v>3149</v>
+        <v>1706</v>
       </c>
       <c r="E23" t="n">
-        <v>20288</v>
+        <v>1854</v>
       </c>
       <c r="F23" t="n">
-        <v>1270</v>
+        <v>113</v>
       </c>
       <c r="G23" t="n">
-        <v>28.63</v>
+        <v>6.38</v>
       </c>
       <c r="H23" t="n">
-        <v>40.33</v>
+        <v>6.87</v>
       </c>
       <c r="I23" t="b">
         <v>0</v>
@@ -1552,16 +1578,16 @@
         <v>0</v>
       </c>
       <c r="K23" t="n">
-        <v>57896</v>
+        <v>29045</v>
       </c>
       <c r="L23" t="n">
-        <v>70838</v>
+        <v>1646</v>
       </c>
       <c r="M23" t="n">
-        <v>1788090</v>
+        <v>227938</v>
       </c>
       <c r="N23" t="n">
-        <v>29.78</v>
+        <v>4.12</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -1572,47 +1598,47 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>California - San Diego</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C24" t="n">
-        <v>17842</v>
+        <v>20623</v>
       </c>
       <c r="D24" t="n">
-        <v>406</v>
+        <v>284</v>
       </c>
       <c r="E24" t="n">
-        <v>642</v>
+        <v>1217</v>
       </c>
       <c r="F24" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G24" t="n">
-        <v>4.52</v>
+        <v>7.64</v>
       </c>
       <c r="H24" t="n">
-        <v>3.76</v>
+        <v>8.119999999999999</v>
       </c>
       <c r="I24" t="b">
         <v>0</v>
       </c>
       <c r="J24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" t="n">
-        <v>14190</v>
+        <v>15936</v>
       </c>
       <c r="L24" t="n">
-        <v>399</v>
+        <v>271</v>
       </c>
       <c r="M24" t="n">
-        <v>166412</v>
+        <v>90860</v>
       </c>
       <c r="N24" t="n">
-        <v>5.04</v>
+        <v>4.77</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -1623,41 +1649,43 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Florida -- Miami-Dade County</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C25" t="n">
-        <v>53974</v>
+        <v>67598</v>
       </c>
       <c r="D25" t="n">
-        <v>1068</v>
+        <v>5941</v>
       </c>
       <c r="E25" t="n">
-        <v>6262</v>
-      </c>
-      <c r="F25" t="inlineStr"/>
+        <v>20291</v>
+      </c>
+      <c r="F25" t="n">
+        <v>2367</v>
+      </c>
       <c r="G25" t="n">
-        <v>20.53</v>
-      </c>
-      <c r="H25" t="inlineStr"/>
+        <v>30.02</v>
+      </c>
+      <c r="H25" t="n">
+        <v>39.84</v>
+      </c>
       <c r="I25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" t="b">
-        <v>1</v>
-      </c>
-      <c r="K25" t="n">
-        <v>30505</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="n">
-        <v>481976</v>
+        <v>1375424</v>
       </c>
       <c r="N25" t="n">
-        <v>17.75</v>
+        <v>13.81</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -1668,26 +1696,30 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Florida -- Orange County</t>
+          <t>California</t>
         </is>
       </c>
       <c r="B26" s="2" t="n">
         <v>44020</v>
       </c>
       <c r="C26" t="n">
-        <v>15194</v>
+        <v>296499</v>
       </c>
       <c r="D26" t="n">
-        <v>63</v>
+        <v>6602</v>
       </c>
       <c r="E26" t="n">
-        <v>1975</v>
-      </c>
-      <c r="F26" t="inlineStr"/>
+        <v>8336</v>
+      </c>
+      <c r="F26" t="n">
+        <v>593</v>
+      </c>
       <c r="G26" t="n">
-        <v>24.35</v>
-      </c>
-      <c r="H26" t="inlineStr"/>
+        <v>4.4</v>
+      </c>
+      <c r="H26" t="n">
+        <v>9.1</v>
+      </c>
       <c r="I26" t="b">
         <v>0</v>
       </c>
@@ -1695,14 +1727,16 @@
         <v>1</v>
       </c>
       <c r="K26" t="n">
-        <v>8111</v>
-      </c>
-      <c r="L26" t="inlineStr"/>
+        <v>190304</v>
+      </c>
+      <c r="L26" t="n">
+        <v>6520</v>
+      </c>
       <c r="M26" t="n">
-        <v>277193</v>
+        <v>2267875</v>
       </c>
       <c r="N26" t="n">
-        <v>20.98</v>
+        <v>5.79</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -1713,98 +1747,80 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>North Carolina</t>
-        </is>
-      </c>
-      <c r="B27" s="2" t="n">
-        <v>44020</v>
-      </c>
-      <c r="C27" t="n">
-        <v>77310</v>
-      </c>
-      <c r="D27" t="n">
-        <v>1441</v>
-      </c>
-      <c r="E27" t="n">
-        <v>12526</v>
-      </c>
-      <c r="F27" t="n">
-        <v>457</v>
-      </c>
-      <c r="G27" t="n">
-        <v>23.74</v>
-      </c>
-      <c r="H27" t="n">
-        <v>32.88</v>
-      </c>
+          <t>Indiana</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
       <c r="I27" t="b">
         <v>0</v>
       </c>
       <c r="J27" t="b">
-        <v>1</v>
-      </c>
-      <c r="K27" t="n">
-        <v>52756</v>
-      </c>
-      <c r="L27" t="n">
-        <v>1390</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
       <c r="M27" t="n">
-        <v>2179622</v>
+        <v>619472</v>
       </c>
       <c r="N27" t="n">
-        <v>21.46</v>
+        <v>9.33</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... KeyError("None of ['RACE'] are in the columns")</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>California - Los Angeles</t>
+          <t>Alaska</t>
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>44019</v>
+        <v>44021</v>
       </c>
       <c r="C28" t="n">
-        <v>123004</v>
+        <v>1272</v>
       </c>
       <c r="D28" t="n">
-        <v>3642</v>
+        <v>17</v>
       </c>
       <c r="E28" t="n">
-        <v>3310</v>
+        <v>30</v>
       </c>
       <c r="F28" t="n">
-        <v>372</v>
+        <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>4.74</v>
+        <v>1.36</v>
       </c>
       <c r="H28" t="n">
-        <v>10.98</v>
+        <v>0</v>
       </c>
       <c r="I28" t="b">
         <v>0</v>
       </c>
       <c r="J28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" t="n">
-        <v>69866</v>
+        <v>2199</v>
       </c>
       <c r="L28" t="n">
-        <v>3389</v>
+        <v>34</v>
       </c>
       <c r="M28" t="n">
-        <v>823987</v>
+        <v>24129</v>
       </c>
       <c r="N28" t="n">
-        <v>8.16</v>
+        <v>3.27</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -1815,39 +1831,47 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Montana</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C29" t="n">
-        <v>1371</v>
+        <v>33908</v>
       </c>
       <c r="D29" t="n">
-        <v>23</v>
+        <v>809</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
-      </c>
-      <c r="F29" t="inlineStr"/>
+        <v>5730</v>
+      </c>
+      <c r="F29" t="n">
+        <v>192</v>
+      </c>
       <c r="G29" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="H29" t="inlineStr"/>
+        <v>18.77</v>
+      </c>
+      <c r="H29" t="n">
+        <v>24.06</v>
+      </c>
       <c r="I29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="b">
         <v>1</v>
       </c>
-      <c r="K29" t="inlineStr"/>
-      <c r="L29" t="inlineStr"/>
+      <c r="K29" t="n">
+        <v>30532</v>
+      </c>
+      <c r="L29" t="n">
+        <v>798</v>
+      </c>
       <c r="M29" t="n">
-        <v>4630</v>
+        <v>368744</v>
       </c>
       <c r="N29" t="n">
-        <v>0.44</v>
+        <v>6.38</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -1858,29 +1882,29 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Virginia</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C30" t="n">
-        <v>67375</v>
+        <v>106727</v>
       </c>
       <c r="D30" t="n">
-        <v>1905</v>
+        <v>2930</v>
       </c>
       <c r="E30" t="n">
-        <v>9967</v>
+        <v>28790</v>
       </c>
       <c r="F30" t="n">
-        <v>429</v>
+        <v>1375</v>
       </c>
       <c r="G30" t="n">
-        <v>14.79</v>
+        <v>26.98</v>
       </c>
       <c r="H30" t="n">
-        <v>22.52</v>
+        <v>46.93</v>
       </c>
       <c r="I30" t="b">
         <v>1</v>
@@ -1891,10 +1915,10 @@
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="n">
-        <v>1613285</v>
+        <v>3239300</v>
       </c>
       <c r="N30" t="n">
-        <v>19.17</v>
+        <v>31.46</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -1905,98 +1929,76 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Rhode Island</t>
-        </is>
-      </c>
-      <c r="B31" s="2" t="n">
-        <v>44015</v>
-      </c>
-      <c r="C31" t="n">
-        <v>16491</v>
-      </c>
-      <c r="D31" t="n">
-        <v>960</v>
-      </c>
-      <c r="E31" t="n">
-        <v>1592</v>
-      </c>
-      <c r="F31" t="n">
-        <v>48</v>
-      </c>
-      <c r="G31" t="n">
-        <v>12.29</v>
-      </c>
-      <c r="H31" t="n">
-        <v>6.14</v>
-      </c>
+          <t>Washington</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
       <c r="I31" t="b">
         <v>0</v>
       </c>
       <c r="J31" t="b">
         <v>0</v>
       </c>
-      <c r="K31" t="n">
-        <v>12950</v>
-      </c>
-      <c r="L31" t="n">
-        <v>782</v>
-      </c>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
       <c r="M31" t="n">
-        <v>69254</v>
+        <v>269854</v>
       </c>
       <c r="N31" t="n">
-        <v>6.55</v>
+        <v>3.7</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... AttributeError("'NoneType' object has no attribute 'groups'")</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>Washington, DC</t>
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C32" t="n">
-        <v>20425</v>
+        <v>10679</v>
       </c>
       <c r="D32" t="n">
-        <v>282</v>
+        <v>568</v>
       </c>
       <c r="E32" t="n">
-        <v>1205</v>
+        <v>5266</v>
       </c>
       <c r="F32" t="n">
-        <v>21</v>
+        <v>421</v>
       </c>
       <c r="G32" t="n">
-        <v>7.63</v>
+        <v>49.31</v>
       </c>
       <c r="H32" t="n">
-        <v>7.72</v>
+        <v>74.12</v>
       </c>
       <c r="I32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" t="b">
         <v>1</v>
       </c>
-      <c r="K32" t="n">
-        <v>15786</v>
-      </c>
-      <c r="L32" t="n">
-        <v>272</v>
-      </c>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
       <c r="M32" t="n">
-        <v>90860</v>
+        <v>321317</v>
       </c>
       <c r="N32" t="n">
-        <v>4.77</v>
+        <v>46.94</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2007,43 +2009,43 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Delaware</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C33" t="n">
-        <v>103890</v>
+        <v>12531</v>
       </c>
       <c r="D33" t="n">
-        <v>2922</v>
+        <v>517</v>
       </c>
       <c r="E33" t="n">
-        <v>28382</v>
+        <v>3212</v>
       </c>
       <c r="F33" t="n">
-        <v>1372</v>
+        <v>132</v>
       </c>
       <c r="G33" t="n">
-        <v>27.32</v>
+        <v>25.63</v>
       </c>
       <c r="H33" t="n">
-        <v>46.95</v>
+        <v>25.53</v>
       </c>
       <c r="I33" t="b">
         <v>1</v>
       </c>
       <c r="J33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
       <c r="M33" t="n">
-        <v>3239300</v>
+        <v>209892</v>
       </c>
       <c r="N33" t="n">
-        <v>31.46</v>
+        <v>22.11</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2054,47 +2056,41 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Wisconsin -- Milwaukee</t>
+          <t>Maine</t>
         </is>
       </c>
       <c r="B34" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C34" t="n">
-        <v>12834</v>
+        <v>3486</v>
       </c>
       <c r="D34" t="n">
-        <v>358</v>
+        <v>111</v>
       </c>
       <c r="E34" t="n">
-        <v>3731</v>
-      </c>
-      <c r="F34" t="n">
-        <v>145</v>
-      </c>
+        <v>809</v>
+      </c>
+      <c r="F34" t="inlineStr"/>
       <c r="G34" t="n">
-        <v>31.32</v>
-      </c>
-      <c r="H34" t="n">
-        <v>40.5</v>
-      </c>
+        <v>26.23</v>
+      </c>
+      <c r="H34" t="inlineStr"/>
       <c r="I34" t="b">
         <v>0</v>
       </c>
       <c r="J34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K34" t="n">
-        <v>11914</v>
-      </c>
-      <c r="L34" t="n">
-        <v>358</v>
-      </c>
+        <v>3084</v>
+      </c>
+      <c r="L34" t="inlineStr"/>
       <c r="M34" t="n">
-        <v>252321</v>
+        <v>17881</v>
       </c>
       <c r="N34" t="n">
-        <v>26.44</v>
+        <v>1.34</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -2105,76 +2101,62 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Idaho</t>
-        </is>
-      </c>
-      <c r="B35" s="2" t="n">
-        <v>44020</v>
-      </c>
-      <c r="C35" t="n">
-        <v>8969</v>
-      </c>
-      <c r="D35" t="n">
-        <v>98</v>
-      </c>
-      <c r="E35" t="n">
-        <v>134</v>
-      </c>
-      <c r="F35" t="n">
-        <v>1</v>
-      </c>
-      <c r="G35" t="n">
-        <v>1.49</v>
-      </c>
-      <c r="H35" t="n">
-        <v>1.02</v>
-      </c>
+          <t>Iowa</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
       <c r="I35" t="b">
         <v>0</v>
       </c>
       <c r="J35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
       <c r="M35" t="n">
-        <v>11536</v>
+        <v>109911</v>
       </c>
       <c r="N35" t="n">
-        <v>0.68</v>
+        <v>3.51</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... ValueError('Unable to parse "Reported Deaths In Adair : No Data" as int')</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Pennsylvania</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C36" t="n">
-        <v>89515</v>
+        <v>79349</v>
       </c>
       <c r="D36" t="n">
-        <v>6812</v>
+        <v>1461</v>
       </c>
       <c r="E36" t="n">
-        <v>11886</v>
+        <v>12925</v>
       </c>
       <c r="F36" t="n">
-        <v>1426</v>
+        <v>461</v>
       </c>
       <c r="G36" t="n">
-        <v>30.04</v>
+        <v>23.8</v>
       </c>
       <c r="H36" t="n">
-        <v>21.68</v>
+        <v>32.72</v>
       </c>
       <c r="I36" t="b">
         <v>0</v>
@@ -2183,16 +2165,16 @@
         <v>1</v>
       </c>
       <c r="K36" t="n">
-        <v>39564</v>
+        <v>54318</v>
       </c>
       <c r="L36" t="n">
-        <v>6579</v>
+        <v>1409</v>
       </c>
       <c r="M36" t="n">
-        <v>1423319</v>
+        <v>2179622</v>
       </c>
       <c r="N36" t="n">
-        <v>11.13</v>
+        <v>21.46</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -2203,47 +2185,43 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C37" t="n">
-        <v>35116</v>
+        <v>150450</v>
       </c>
       <c r="D37" t="n">
-        <v>1704</v>
+        <v>7119</v>
       </c>
       <c r="E37" t="n">
-        <v>1840</v>
+        <v>25255</v>
       </c>
       <c r="F37" t="n">
-        <v>111</v>
+        <v>1971</v>
       </c>
       <c r="G37" t="n">
-        <v>6.39</v>
+        <v>16.79</v>
       </c>
       <c r="H37" t="n">
-        <v>6.75</v>
+        <v>27.69</v>
       </c>
       <c r="I37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" t="b">
         <v>0</v>
       </c>
-      <c r="K37" t="n">
-        <v>28809</v>
-      </c>
-      <c r="L37" t="n">
-        <v>1644</v>
-      </c>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
       <c r="M37" t="n">
-        <v>227938</v>
+        <v>1824125</v>
       </c>
       <c r="N37" t="n">
-        <v>4.12</v>
+        <v>14.23</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -2254,47 +2232,43 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Idaho</t>
         </is>
       </c>
       <c r="B38" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C38" t="n">
-        <v>37941</v>
+        <v>9428</v>
       </c>
       <c r="D38" t="n">
-        <v>1394</v>
+        <v>98</v>
       </c>
       <c r="E38" t="n">
-        <v>1478</v>
+        <v>139</v>
       </c>
       <c r="F38" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="G38" t="n">
-        <v>5.48</v>
+        <v>1.47</v>
       </c>
       <c r="H38" t="n">
-        <v>3.4</v>
+        <v>1.02</v>
       </c>
       <c r="I38" t="b">
         <v>0</v>
       </c>
       <c r="J38" t="b">
-        <v>0</v>
-      </c>
-      <c r="K38" t="n">
-        <v>26965</v>
-      </c>
-      <c r="L38" t="n">
-        <v>1323</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
       <c r="M38" t="n">
-        <v>269854</v>
+        <v>11536</v>
       </c>
       <c r="N38" t="n">
-        <v>3.7</v>
+        <v>0.68</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -2305,43 +2279,43 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="B39" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C39" t="n">
-        <v>220492</v>
+        <v>40163</v>
       </c>
       <c r="D39" t="n">
-        <v>3889</v>
+        <v>1490</v>
       </c>
       <c r="E39" t="n">
-        <v>28460</v>
+        <v>8168</v>
       </c>
       <c r="F39" t="n">
-        <v>764</v>
+        <v>143</v>
       </c>
       <c r="G39" t="n">
-        <v>12.91</v>
+        <v>20.34</v>
       </c>
       <c r="H39" t="n">
-        <v>19.65</v>
+        <v>9.6</v>
       </c>
       <c r="I39" t="b">
         <v>1</v>
       </c>
       <c r="J39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
       <c r="M39" t="n">
-        <v>3316376</v>
+        <v>342186</v>
       </c>
       <c r="N39" t="n">
-        <v>16.1</v>
+        <v>6.19</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -2352,29 +2326,29 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="B40" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C40" t="n">
-        <v>67153</v>
+        <v>110897</v>
       </c>
       <c r="D40" t="n">
-        <v>5934</v>
+        <v>8268</v>
       </c>
       <c r="E40" t="n">
-        <v>20210</v>
+        <v>10442</v>
       </c>
       <c r="F40" t="n">
-        <v>2367</v>
+        <v>679</v>
       </c>
       <c r="G40" t="n">
-        <v>30.1</v>
+        <v>9.42</v>
       </c>
       <c r="H40" t="n">
-        <v>39.89</v>
+        <v>8.210000000000001</v>
       </c>
       <c r="I40" t="b">
         <v>1</v>
@@ -2385,10 +2359,10 @@
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="n">
-        <v>1375424</v>
+        <v>510558</v>
       </c>
       <c r="N40" t="n">
-        <v>13.81</v>
+        <v>7.48</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -2399,43 +2373,47 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Mississippi</t>
+          <t>Wisconsin -- Milwaukee</t>
         </is>
       </c>
       <c r="B41" s="2" t="n">
-        <v>44019</v>
+        <v>44021</v>
       </c>
       <c r="C41" t="n">
-        <v>32888</v>
+        <v>13096</v>
       </c>
       <c r="D41" t="n">
-        <v>1188</v>
+        <v>358</v>
       </c>
       <c r="E41" t="n">
-        <v>15720</v>
+        <v>3792</v>
       </c>
       <c r="F41" t="n">
-        <v>595</v>
+        <v>145</v>
       </c>
       <c r="G41" t="n">
-        <v>47.8</v>
+        <v>31.23</v>
       </c>
       <c r="H41" t="n">
-        <v>50.08</v>
+        <v>40.5</v>
       </c>
       <c r="I41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" t="b">
-        <v>1</v>
-      </c>
-      <c r="K41" t="inlineStr"/>
-      <c r="L41" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K41" t="n">
+        <v>12144</v>
+      </c>
+      <c r="L41" t="n">
+        <v>358</v>
+      </c>
       <c r="M41" t="n">
-        <v>1125834</v>
+        <v>252321</v>
       </c>
       <c r="N41" t="n">
-        <v>37.67</v>
+        <v>26.44</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -2446,43 +2424,47 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Delaware</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="B42" s="2" t="n">
-        <v>44020</v>
+        <v>44009</v>
       </c>
       <c r="C42" t="n">
-        <v>12462</v>
+        <v>20261</v>
       </c>
       <c r="D42" t="n">
-        <v>515</v>
+        <v>996</v>
       </c>
       <c r="E42" t="n">
-        <v>3197</v>
+        <v>5758</v>
       </c>
       <c r="F42" t="n">
-        <v>131</v>
+        <v>246</v>
       </c>
       <c r="G42" t="n">
-        <v>25.65</v>
+        <v>49.66</v>
       </c>
       <c r="H42" t="n">
-        <v>25.44</v>
+        <v>38.56</v>
       </c>
       <c r="I42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" t="b">
-        <v>0</v>
-      </c>
-      <c r="K42" t="inlineStr"/>
-      <c r="L42" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K42" t="n">
+        <v>11594</v>
+      </c>
+      <c r="L42" t="n">
+        <v>638</v>
+      </c>
       <c r="M42" t="n">
-        <v>209892</v>
+        <v>704896</v>
       </c>
       <c r="N42" t="n">
-        <v>22.11</v>
+        <v>11.57</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Results from July 09, 2020 07:13:40 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-09.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-09.xlsx
@@ -2235,32 +2235,18 @@
           <t>Idaho</t>
         </is>
       </c>
-      <c r="B38" s="2" t="n">
-        <v>44021</v>
-      </c>
-      <c r="C38" t="n">
-        <v>9428</v>
-      </c>
-      <c r="D38" t="n">
-        <v>98</v>
-      </c>
-      <c r="E38" t="n">
-        <v>139</v>
-      </c>
-      <c r="F38" t="n">
-        <v>1</v>
-      </c>
-      <c r="G38" t="n">
-        <v>1.47</v>
-      </c>
-      <c r="H38" t="n">
-        <v>1.02</v>
-      </c>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
       <c r="I38" t="b">
         <v>0</v>
       </c>
       <c r="J38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
@@ -2272,7 +2258,7 @@
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... TimeoutException('', None, None)</t>
         </is>
       </c>
     </row>

</xml_diff>